<commit_message>
Tilauslista muutettu DataGridViewksi. Tilaus luokan kehitys.
</commit_message>
<xml_diff>
--- a/Projekti_Tyoajanseuranta_ryhma08.xlsx
+++ b/Projekti_Tyoajanseuranta_ryhma08.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>TYÖAJANSEURANTALOMAKE</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Painikkeet logiikkaa</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Tilaus luokka</t>
   </si>
 </sst>
 </file>
@@ -521,13 +527,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,7 +817,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1236,11 +1242,11 @@
       <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
@@ -1293,10 +1299,10 @@
       <c r="G8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="29">
         <v>0.60416666666666663</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="29">
         <v>0.6875</v>
       </c>
     </row>
@@ -1318,10 +1324,10 @@
       <c r="G9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="31">
+      <c r="H9" s="29">
         <v>0.69791666666666663</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="29">
         <v>0.77777777777777779</v>
       </c>
     </row>
@@ -1338,6 +1344,15 @@
         <v>3</v>
       </c>
       <c r="E10" s="25"/>
+      <c r="G10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="29">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="I10" s="29">
+        <v>0.80555555555555547</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
@@ -1352,6 +1367,15 @@
         <v>2</v>
       </c>
       <c r="E11" s="25"/>
+      <c r="G11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="29">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="I11" s="29">
+        <v>0.84027777777777779</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">

</xml_diff>

<commit_message>
Tilauksen tietojen hakeminen kannasta
</commit_message>
<xml_diff>
--- a/Projekti_Tyoajanseuranta_ryhma08.xlsx
+++ b/Projekti_Tyoajanseuranta_ryhma08.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>TYÖAJANSEURANTALOMAKE</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Tilauslistan refresh</t>
+  </si>
+  <si>
+    <t>LataaTilaus kannasta</t>
   </si>
 </sst>
 </file>
@@ -823,7 +826,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1446,6 +1449,9 @@
       <c r="H14" s="29">
         <v>0</v>
       </c>
+      <c r="I14" s="29">
+        <v>5.5555555555555552E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
@@ -1458,6 +1464,12 @@
       <c r="C15" s="23"/>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
+      <c r="G15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="29">
+        <v>0.625</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">

</xml_diff>

<commit_message>
Valmis, tuntilista ajan tasalle
</commit_message>
<xml_diff>
--- a/Projekti_Tyoajanseuranta_ryhma08.xlsx
+++ b/Projekti_Tyoajanseuranta_ryhma08.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>TYÖAJANSEURANTALOMAKE</t>
   </si>
@@ -63,30 +63,6 @@
     <t>Koodin suunnittelu</t>
   </si>
   <si>
-    <t>9: InMemoryAteriaDb</t>
-  </si>
-  <si>
-    <t>10: Poyta-luokka</t>
-  </si>
-  <si>
-    <t>11: InMemoryPoytaDb -luokka</t>
-  </si>
-  <si>
-    <t>12: Asiakas -luokka</t>
-  </si>
-  <si>
-    <t>13: BonusAsiakas-luokka</t>
-  </si>
-  <si>
-    <t>14: InMemoryBonusAsiakasDb-luokka</t>
-  </si>
-  <si>
-    <t>15:Tapahtumantila-enum</t>
-  </si>
-  <si>
-    <t>16: Varaustilanne-enum</t>
-  </si>
-  <si>
     <t>17. Versionhallinnan käytttöönotto</t>
   </si>
   <si>
@@ -111,43 +87,19 @@
     <t>Tilaus / Tilausrivi -luokat</t>
   </si>
   <si>
-    <t>Tilaushallinta luokka</t>
-  </si>
-  <si>
-    <t>Käyttöliittymän toiminnallisuuden koodaus</t>
-  </si>
-  <si>
-    <t>Ohjelmalogiikkaa</t>
-  </si>
-  <si>
-    <t>Alkaen</t>
-  </si>
-  <si>
-    <t>Loppu</t>
-  </si>
-  <si>
-    <t>Painikkeet logiikkaa</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Tilaus luokka</t>
-  </si>
-  <si>
-    <t>Tilauksen lisääminen</t>
-  </si>
-  <si>
-    <t>Tilauslistan refresh</t>
-  </si>
-  <si>
-    <t>LataaTilaus kannasta</t>
-  </si>
-  <si>
-    <t>Tilauksen tallennus</t>
-  </si>
-  <si>
-    <t>Julkaisu</t>
+    <t>Tilauksen lisääminen kantaan</t>
+  </si>
+  <si>
+    <t>Tilauskannan näyttäminen tilauslistassa</t>
+  </si>
+  <si>
+    <t>Tilauksen lataaminen kannasta näkyviin</t>
+  </si>
+  <si>
+    <t>Tilauskanna tallennus tiedostoon</t>
+  </si>
+  <si>
+    <t>Painikkeet ohjelmalogiikkaa</t>
   </si>
 </sst>
 </file>
@@ -829,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1279,7 +1231,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="11">
-        <f t="shared" ref="B7:B33" si="0">SUM(C7:E7)</f>
+        <f t="shared" ref="B7:B21" si="0">SUM(C7:E7)</f>
         <v>2</v>
       </c>
       <c r="C7" s="23"/>
@@ -1289,12 +1241,6 @@
       <c r="E7" s="25">
         <v>1</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
@@ -1311,15 +1257,8 @@
       <c r="E8" s="25">
         <v>2</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="29">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="I8" s="29">
-        <v>0.6875</v>
-      </c>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
@@ -1336,15 +1275,8 @@
       <c r="E9" s="25">
         <v>3</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="29">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="I9" s="29">
-        <v>0.77777777777777779</v>
-      </c>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
@@ -1359,15 +1291,9 @@
         <v>3</v>
       </c>
       <c r="E10" s="25"/>
-      <c r="G10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="29">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="I10" s="29">
-        <v>0.80555555555555547</v>
-      </c>
+      <c r="G10" s="28"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
@@ -1382,184 +1308,156 @@
         <v>2</v>
       </c>
       <c r="E11" s="25"/>
-      <c r="G11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="29">
-        <v>0.80555555555555547</v>
-      </c>
-      <c r="I11" s="29">
-        <v>0.84027777777777779</v>
-      </c>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B12" s="13">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12" s="25"/>
-      <c r="G12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="29">
-        <v>0.84027777777777779</v>
-      </c>
-      <c r="I12" s="29">
-        <v>0.90972222222222221</v>
-      </c>
+      <c r="G12" s="28"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B13" s="13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="25">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="E13" s="25"/>
-      <c r="G13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="29">
-        <v>0.93055555555555547</v>
-      </c>
-      <c r="I13" s="29">
-        <v>0</v>
-      </c>
+      <c r="G13" s="28"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="26" t="s">
-        <v>28</v>
+      <c r="A14" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="B14" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="C14" s="23"/>
-      <c r="D14" s="25"/>
+      <c r="D14" s="25">
+        <v>1.5</v>
+      </c>
       <c r="E14" s="25"/>
-      <c r="G14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="29">
-        <v>0</v>
-      </c>
-      <c r="I14" s="29">
-        <v>5.5555555555555552E-2</v>
-      </c>
+      <c r="G14" s="28"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>11</v>
+      <c r="A15" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="B15" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="C15" s="23"/>
-      <c r="D15" s="25"/>
+      <c r="D15" s="25">
+        <v>1.5</v>
+      </c>
       <c r="E15" s="25"/>
-      <c r="G15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="29">
-        <v>0.625</v>
-      </c>
-      <c r="I15" s="29">
-        <v>0.69444444444444453</v>
-      </c>
+      <c r="G15" s="28"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
-        <v>12</v>
+      <c r="A16" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="B16" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="23"/>
-      <c r="D16" s="25"/>
+      <c r="D16" s="25">
+        <v>1</v>
+      </c>
       <c r="E16" s="25"/>
-      <c r="G16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="29">
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="I16" s="29">
-        <v>0.73611111111111116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>13</v>
+      <c r="H16" s="29"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
+        <v>23</v>
       </c>
       <c r="B17" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C17" s="23"/>
-      <c r="D17" s="25"/>
+      <c r="D17" s="25">
+        <v>4</v>
+      </c>
       <c r="E17" s="25"/>
-      <c r="G17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="29">
-        <v>0.73611111111111116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="26" t="s">
-        <v>14</v>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="B18" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C18" s="23"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D18" s="25">
+        <v>2</v>
+      </c>
+      <c r="E18" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B19" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C19" s="23"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
-        <v>16</v>
+      <c r="D19" s="25">
+        <v>3</v>
+      </c>
+      <c r="E19" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="B20" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="13">
+      <c r="E20" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1567,205 +1465,66 @@
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="13">
-        <f t="shared" si="0"/>
+    <row r="22" spans="1:5" s="19" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="18">
+        <f>SUM(B7:B21)</f>
+        <v>45.5</v>
+      </c>
+      <c r="C22" s="18">
+        <f>SUM(C7:C21)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="13">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="25">
-        <v>2</v>
-      </c>
-      <c r="E23" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="13">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="25">
-        <v>3</v>
-      </c>
-      <c r="E24" s="25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="13">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
-      <c r="B28" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="G28" s="14"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="12"/>
-      <c r="B29" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-    </row>
-    <row r="33" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-    </row>
-    <row r="34" spans="1:5" s="19" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="18">
-        <f>SUM(B7:B33)</f>
-        <v>33</v>
-      </c>
-      <c r="C34" s="18">
-        <f>SUM(C7:C33)</f>
-        <v>0</v>
-      </c>
-      <c r="D34" s="18">
-        <f>SUM(D7:D33)</f>
-        <v>19</v>
-      </c>
-      <c r="E34" s="18">
-        <f>SUM(E7:E33)</f>
+      <c r="D22" s="18">
+        <f>SUM(D7:D21)</f>
+        <v>31.5</v>
+      </c>
+      <c r="E22" s="18">
+        <f>SUM(E7:E21)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-    </row>
-    <row r="36" spans="1:5" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="22"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
+    <row r="23" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+    </row>
+    <row r="24" spans="1:5" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="22"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="22"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="22"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>